<commit_message>
some codebook FUN fixes, minimal example
</commit_message>
<xml_diff>
--- a/inst/extdata/example_scaleInfo.xlsx
+++ b/inst/extdata/example_scaleInfo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">varName</t>
   </si>
@@ -33,6 +33,18 @@
   </si>
   <si>
     <t xml:space="preserve">skala1_item1,skala1_item2,skala1_item3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pv_pooled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pv_1,pv_2,pv_3,pv_4,pv_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pvkat_pooled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pvkat_1,pvkat_2,pvkat_3,pvkat_4,pvkat_5</t>
   </si>
 </sst>
 </file>
@@ -390,6 +402,30 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4"/>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
[createScaleInfo] Separate items of a scale and imputation information
Information on imputations and items of a scale was initially stored in the same column. This decreased understandability in code and in usage, and made it impossible to have an imputed scale with items.

#28
</commit_message>
<xml_diff>
--- a/inst/extdata/example_scaleInfo.xlsx
+++ b/inst/extdata/example_scaleInfo.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">varName</t>
   </si>
@@ -26,6 +26,9 @@
     <t xml:space="preserve">Items_der_Skala</t>
   </si>
   <si>
+    <t xml:space="preserve">Imputationen</t>
+  </si>
+  <si>
     <t xml:space="preserve">skala1</t>
   </si>
   <si>
@@ -33,6 +36,9 @@
   </si>
   <si>
     <t xml:space="preserve">skala1_item1,skala1_item2,skala1_item3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
   </si>
   <si>
     <t xml:space="preserve">pv_pooled</t>
@@ -389,41 +395,53 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2"/>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>